<commit_message>
update to keep JP2 as-is 3x2P header for power source selection.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="248">
   <si>
     <t xml:space="preserve">assembly_no</t>
   </si>
@@ -73,7 +73,7 @@
     <t xml:space="preserve">Comments</t>
   </si>
   <si>
-    <t xml:space="preserve">WRAITH.001.Z1</t>
+    <t xml:space="preserve">WRAITH.001.Z2</t>
   </si>
   <si>
     <t xml:space="preserve">ASSY,PCB,SPECTER,WRAITH</t>
@@ -109,17 +109,13 @@
     <t xml:space="preserve">JP2</t>
   </si>
   <si>
-    <t xml:space="preserve">TSM-102-01-x-SV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CONN,HEADER,SM,2P</t>
+    <t xml:space="preserve">TSM-103-01-x-DV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONN,HEADER,SM,3x2P</t>
   </si>
   <si>
     <t xml:space="preserve">SAMTEC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEL JP1, JP5
-ADD JP2</t>
   </si>
   <si>
     <t xml:space="preserve">TP1, TP2, TP3, TP4, TP5, TP6, TP7</t>
@@ -796,6 +792,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -817,6 +814,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -896,11 +894,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -996,10 +994,10 @@
   <dimension ref="A1:P96"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="37.74"/>
@@ -1011,9 +1009,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="25.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="26.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="8.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="35.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="35.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="8.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="27.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="27.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="14" style="1" width="22.28"/>
   </cols>
   <sheetData>
@@ -1086,7 +1084,7 @@
       <c r="F2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="4" t="n">
+      <c r="G2" s="3" t="n">
         <v>1</v>
       </c>
       <c r="H2" s="3" t="s">
@@ -1129,10 +1127,10 @@
       <c r="E3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="4" t="n">
+      <c r="G3" s="3" t="n">
         <v>4</v>
       </c>
       <c r="H3" s="1" t="s">
@@ -1141,11 +1139,11 @@
       <c r="I3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="P3" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
@@ -1153,18 +1151,18 @@
         <v>17</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="D4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="4" t="n">
+      <c r="G4" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H4" s="1" t="s">
@@ -1179,9 +1177,8 @@
       <c r="K4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="P4" s="5" t="s">
-        <v>31</v>
-      </c>
+      <c r="L4" s="0"/>
+      <c r="M4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
@@ -1194,22 +1191,22 @@
         <v>9</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="G5" s="4" t="n">
-        <v>7</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1223,26 +1220,26 @@
         <v>11</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="3"/>
+      <c r="G6" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="K6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1256,31 +1253,31 @@
         <v>12</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="G7" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I7" s="1" t="s">
+      <c r="J7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M7" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1294,28 +1291,28 @@
         <v>13</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="G8" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G8" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I8" s="1" t="s">
+      <c r="J8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1329,28 +1326,28 @@
         <v>15</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="J9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1364,31 +1361,31 @@
         <v>18</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="G10" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="G10" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>30</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="P10" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1402,22 +1399,22 @@
         <v>20</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="G11" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="H11" s="1" t="s">
+      <c r="I11" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1431,22 +1428,22 @@
         <v>21</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" s="4" t="s">
+      <c r="G12" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="G12" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="H12" s="1" t="s">
+      <c r="I12" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1460,28 +1457,28 @@
         <v>22</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I13" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F13" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="G13" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="I13" s="1" t="s">
+      <c r="J13" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="J13" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="K13" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1495,22 +1492,22 @@
         <v>24</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G14" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="G14" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="I14" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1524,34 +1521,34 @@
         <v>26</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="F15" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="G15" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I15" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G15" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I15" s="1" t="s">
+      <c r="J15" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="K15" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="K15" s="1" t="s">
+      <c r="M15" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="M15" s="1" t="s">
+      <c r="P15" s="4" t="s">
         <v>79</v>
-      </c>
-      <c r="P15" s="5" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1565,28 +1562,28 @@
         <v>27</v>
       </c>
       <c r="D16" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="F16" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="G16" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I16" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="G16" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="I16" s="1" t="s">
+      <c r="J16" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="K16" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1600,31 +1597,31 @@
         <v>28</v>
       </c>
       <c r="D17" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="F17" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="G17" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="P17" s="4" t="s">
         <v>88</v>
-      </c>
-      <c r="G17" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="P17" s="5" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1638,34 +1635,34 @@
         <v>29</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E18" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="F18" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="G18" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="G18" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="H18" s="1" t="s">
+      <c r="I18" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="J18" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="K18" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M18" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="K18" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="M18" s="1" t="s">
+      <c r="P18" s="7" t="s">
         <v>96</v>
-      </c>
-      <c r="P18" s="7" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1679,25 +1676,25 @@
         <v>30</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="F19" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="G19" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I19" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="G19" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I19" s="1" t="s">
+      <c r="J19" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="P19" s="6" t="s">
         <v>102</v>
-      </c>
-      <c r="P19" s="6" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1711,28 +1708,28 @@
         <v>32</v>
       </c>
       <c r="D20" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G20" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I20" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="F20" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G20" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="J20" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1746,28 +1743,28 @@
         <v>33</v>
       </c>
       <c r="D21" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="G21" s="4" t="n">
+      <c r="G21" s="3" t="n">
         <v>1</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1781,28 +1778,28 @@
         <v>35</v>
       </c>
       <c r="D22" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="F22" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="G22" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="G22" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="H22" s="1" t="s">
+      <c r="J22" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J22" s="1" t="s">
+      <c r="K22" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="P22" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="P22" s="1" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1816,25 +1813,25 @@
         <v>37</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F23" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="G23" s="4" t="n">
+      <c r="F23" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G23" s="3" t="n">
         <v>2</v>
       </c>
       <c r="H23" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="P23" s="4" t="s">
         <v>117</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="P23" s="5" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1848,37 +1845,37 @@
         <v>38</v>
       </c>
       <c r="D24" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="F24" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G24" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I24" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="F24" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="G24" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="I24" s="1" t="s">
+      <c r="J24" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="J24" s="1" t="s">
+      <c r="K24" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="K24" s="1" t="s">
+      <c r="L24" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="L24" s="1" t="s">
+      <c r="M24" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="P24" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="M24" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="P24" s="1" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1892,34 +1889,34 @@
         <v>39</v>
       </c>
       <c r="D25" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="F25" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G25" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I25" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="F25" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="G25" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="I25" s="1" t="s">
+      <c r="J25" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K25" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="J25" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>129</v>
-      </c>
       <c r="L25" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1933,25 +1930,25 @@
         <v>41</v>
       </c>
       <c r="D26" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F26" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="G26" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H26" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="G26" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="H26" s="1" t="s">
+      <c r="I26" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="I26" s="1" t="s">
-        <v>133</v>
-      </c>
       <c r="J26" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1965,25 +1962,25 @@
         <v>43</v>
       </c>
       <c r="D27" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F27" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F27" s="4" t="s">
+      <c r="G27" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="H27" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="G27" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="H27" s="1" t="s">
+      <c r="I27" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="I27" s="1" t="s">
+      <c r="P27" s="4" t="s">
         <v>137</v>
-      </c>
-      <c r="P27" s="5" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1997,22 +1994,22 @@
         <v>44</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F28" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="G28" s="4" t="n">
+      <c r="F28" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G28" s="3" t="n">
         <v>1</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2026,22 +2023,22 @@
         <v>45</v>
       </c>
       <c r="D29" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="F29" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="F29" s="4" t="s">
+      <c r="G29" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="H29" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G29" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="H29" s="1" t="s">
+      <c r="I29" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2055,22 +2052,22 @@
         <v>46</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F30" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="G30" s="4" t="n">
+      <c r="F30" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="G30" s="3" t="n">
         <v>1</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2084,25 +2081,25 @@
         <v>48</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E31" s="1" t="n">
         <v>475900001</v>
       </c>
-      <c r="F31" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="G31" s="4" t="n">
+      <c r="F31" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G31" s="3" t="n">
         <v>1</v>
       </c>
       <c r="H31" s="1" t="n">
         <v>475900001</v>
       </c>
       <c r="I31" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="J31" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="J31" s="1" t="s">
-        <v>150</v>
       </c>
       <c r="K31" s="1" t="n">
         <v>475900001</v>
@@ -2119,28 +2116,28 @@
         <v>49</v>
       </c>
       <c r="D32" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="F32" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="F32" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="G32" s="4" t="n">
+      <c r="G32" s="3" t="n">
         <v>1</v>
       </c>
       <c r="H32" s="1" t="n">
         <v>9013</v>
       </c>
       <c r="I32" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="P32" s="4" t="s">
         <v>154</v>
-      </c>
-      <c r="K32" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="P32" s="5" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2154,15 +2151,15 @@
         <v>50</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F33" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="G33" s="4" t="n">
+      <c r="F33" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="G33" s="3" t="n">
         <v>1</v>
       </c>
       <c r="H33" s="1" t="n">
@@ -2183,15 +2180,15 @@
         <v>51</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F34" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="G34" s="4" t="n">
+      <c r="F34" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="G34" s="3" t="n">
         <v>4</v>
       </c>
       <c r="H34" s="1" t="n">
@@ -2212,15 +2209,15 @@
         <v>52</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F35" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="G35" s="4" t="n">
+      <c r="F35" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="G35" s="3" t="n">
         <v>2</v>
       </c>
       <c r="H35" s="1" t="n">
@@ -2229,8 +2226,8 @@
       <c r="I35" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="P35" s="5" t="s">
-        <v>162</v>
+      <c r="P35" s="4" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2244,15 +2241,15 @@
         <v>53</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F36" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="G36" s="4" t="n">
+      <c r="F36" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="G36" s="3" t="n">
         <v>1</v>
       </c>
       <c r="H36" s="1" t="n">
@@ -2261,8 +2258,8 @@
       <c r="I36" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="P36" s="5" t="s">
-        <v>165</v>
+      <c r="P36" s="4" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2276,25 +2273,25 @@
         <v>56</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E37" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F37" s="4" t="s">
+      <c r="F37" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="G37" s="3" t="n">
+        <v>46</v>
+      </c>
+      <c r="H37" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="G37" s="4" t="n">
-        <v>46</v>
-      </c>
-      <c r="H37" s="1" t="s">
+      <c r="I37" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="I37" s="6" t="s">
+      <c r="P37" s="4" t="s">
         <v>169</v>
-      </c>
-      <c r="P37" s="5" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2308,22 +2305,22 @@
         <v>57</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F38" s="4" t="s">
+      <c r="F38" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="G38" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H38" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="G38" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="H38" s="1" t="s">
+      <c r="I38" s="6" t="s">
         <v>173</v>
-      </c>
-      <c r="I38" s="6" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2337,25 +2334,25 @@
         <v>58</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F39" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="G39" s="4" t="n">
+      <c r="F39" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="G39" s="3" t="n">
         <v>1</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="P39" s="5" t="s">
-        <v>177</v>
+      <c r="P39" s="4" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2369,19 +2366,19 @@
         <v>61</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F40" s="4" t="s">
+      <c r="F40" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="G40" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="H40" s="1" t="s">
         <v>179</v>
-      </c>
-      <c r="G40" s="4" t="n">
-        <v>7</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>180</v>
       </c>
       <c r="I40" s="1" t="s">
         <v>25</v>
@@ -2398,19 +2395,19 @@
         <v>65</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F41" s="4" t="s">
+      <c r="F41" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="G41" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="H41" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="G41" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2424,22 +2421,22 @@
         <v>66</v>
       </c>
       <c r="D42" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E42" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="E42" s="6" t="s">
+      <c r="F42" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="F42" s="4" t="s">
+      <c r="G42" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H42" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="G42" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="H42" s="1" t="s">
+      <c r="I42" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="I42" s="1" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2453,25 +2450,25 @@
         <v>67</v>
       </c>
       <c r="D43" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="F43" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="E43" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="F43" s="4" t="s">
+      <c r="G43" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="H43" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="G43" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="H43" s="1" t="s">
+      <c r="I43" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="I43" s="1" t="s">
+      <c r="P43" s="4" t="s">
         <v>192</v>
-      </c>
-      <c r="P43" s="5" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2485,25 +2482,25 @@
         <v>69</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F44" s="4" t="s">
+      <c r="F44" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="G44" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="H44" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="G44" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="H44" s="1" t="s">
+      <c r="I44" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="I44" s="1" t="s">
+      <c r="P44" s="4" t="s">
         <v>197</v>
-      </c>
-      <c r="P44" s="5" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2517,28 +2514,28 @@
         <v>70</v>
       </c>
       <c r="D45" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="E45" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="F45" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="F45" s="4" t="s">
+      <c r="G45" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="H45" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="G45" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>202</v>
       </c>
       <c r="I45" s="1" t="s">
         <v>25</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2552,31 +2549,31 @@
         <v>71</v>
       </c>
       <c r="D46" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="E46" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="E46" s="6" t="s">
+      <c r="F46" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="F46" s="4" t="s">
+      <c r="G46" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="I46" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="P46" s="4" t="s">
         <v>206</v>
-      </c>
-      <c r="G46" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="I46" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="J46" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="K46" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="P46" s="5" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2590,15 +2587,15 @@
         <v>72</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F47" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="G47" s="4" t="n">
+      <c r="F47" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="G47" s="3" t="n">
         <v>1</v>
       </c>
       <c r="H47" s="1" t="n">
@@ -2619,22 +2616,22 @@
         <v>73</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F48" s="4" t="s">
+      <c r="F48" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="G48" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="H48" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="G48" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="H48" s="1" t="s">
-        <v>212</v>
-      </c>
       <c r="I48" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2648,22 +2645,22 @@
         <v>74</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F49" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="G49" s="4" t="n">
+      <c r="F49" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="G49" s="3" t="n">
         <v>1</v>
       </c>
       <c r="H49" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="I49" s="1" t="s">
         <v>214</v>
-      </c>
-      <c r="I49" s="1" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2677,22 +2674,22 @@
         <v>75</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F50" s="4" t="s">
+      <c r="F50" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="G50" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H50" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="G50" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="H50" s="1" t="s">
+      <c r="I50" s="1" t="s">
         <v>218</v>
-      </c>
-      <c r="I50" s="1" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2706,22 +2703,22 @@
         <v>76</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F51" s="4" t="s">
+      <c r="F51" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="G51" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H51" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="G51" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>222</v>
-      </c>
       <c r="I51" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2735,22 +2732,22 @@
         <v>77</v>
       </c>
       <c r="D52" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="F52" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="E52" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="F52" s="4" t="s">
+      <c r="G52" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="H52" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="G52" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="H52" s="1" t="s">
-        <v>225</v>
-      </c>
       <c r="I52" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2764,25 +2761,25 @@
         <v>78</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F53" s="4" t="s">
+      <c r="F53" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="G53" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="H53" s="1" t="s">
         <v>227</v>
-      </c>
-      <c r="G53" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="H53" s="1" t="s">
-        <v>228</v>
       </c>
       <c r="I53" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="P53" s="5" t="s">
-        <v>229</v>
+      <c r="P53" s="4" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2796,22 +2793,22 @@
         <v>79</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F54" s="4" t="s">
+      <c r="F54" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="G54" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="H54" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="G54" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="H54" s="1" t="s">
-        <v>232</v>
-      </c>
       <c r="I54" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2825,19 +2822,19 @@
         <v>80</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F55" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="G55" s="4" t="n">
+      <c r="F55" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="G55" s="3" t="n">
         <v>4</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2851,22 +2848,22 @@
         <v>81</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F56" s="4" t="s">
+      <c r="F56" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="G56" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="H56" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="G56" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="H56" s="1" t="s">
-        <v>237</v>
-      </c>
       <c r="I56" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2880,22 +2877,22 @@
         <v>85</v>
       </c>
       <c r="D57" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="F57" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="E57" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="F57" s="4" t="s">
+      <c r="G57" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="H57" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="G57" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="H57" s="1" t="s">
-        <v>240</v>
-      </c>
       <c r="I57" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2909,25 +2906,25 @@
         <v>86</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F58" s="4" t="s">
+      <c r="F58" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="G58" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="H58" s="1" t="s">
         <v>242</v>
-      </c>
-      <c r="G58" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="H58" s="1" t="s">
-        <v>243</v>
       </c>
       <c r="I58" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="P58" s="5" t="s">
-        <v>244</v>
+      <c r="P58" s="4" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2941,15 +2938,15 @@
         <v>87</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F59" s="4" t="s">
-        <v>246</v>
-      </c>
-      <c r="G59" s="4" t="n">
+      <c r="F59" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="G59" s="3" t="n">
         <v>14</v>
       </c>
       <c r="H59" s="1" t="n">
@@ -2958,589 +2955,589 @@
       <c r="I59" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="P59" s="5" t="s">
-        <v>247</v>
+      <c r="P59" s="4" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="4"/>
-      <c r="B60" s="4"/>
-      <c r="C60" s="4"/>
-      <c r="D60" s="4"/>
-      <c r="E60" s="4"/>
-      <c r="F60" s="4"/>
-      <c r="G60" s="4"/>
-      <c r="H60" s="4"/>
-      <c r="I60" s="4"/>
-      <c r="J60" s="4"/>
-      <c r="K60" s="4"/>
-      <c r="L60" s="4"/>
-      <c r="M60" s="4"/>
-      <c r="N60" s="4"/>
-      <c r="O60" s="4"/>
-      <c r="P60" s="4"/>
+      <c r="A60" s="3"/>
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
+      <c r="F60" s="3"/>
+      <c r="G60" s="3"/>
+      <c r="H60" s="3"/>
+      <c r="I60" s="3"/>
+      <c r="J60" s="3"/>
+      <c r="K60" s="3"/>
+      <c r="L60" s="3"/>
+      <c r="M60" s="3"/>
+      <c r="N60" s="3"/>
+      <c r="O60" s="3"/>
+      <c r="P60" s="3"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="4"/>
-      <c r="B61" s="4"/>
-      <c r="C61" s="4"/>
-      <c r="D61" s="4"/>
-      <c r="E61" s="4"/>
-      <c r="F61" s="4"/>
-      <c r="G61" s="4"/>
-      <c r="H61" s="4"/>
-      <c r="I61" s="4"/>
-      <c r="J61" s="4"/>
-      <c r="K61" s="4"/>
-      <c r="L61" s="4"/>
-      <c r="M61" s="4"/>
-      <c r="N61" s="4"/>
-      <c r="O61" s="4"/>
-      <c r="P61" s="4"/>
+      <c r="A61" s="3"/>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3"/>
+      <c r="G61" s="3"/>
+      <c r="H61" s="3"/>
+      <c r="I61" s="3"/>
+      <c r="J61" s="3"/>
+      <c r="K61" s="3"/>
+      <c r="L61" s="3"/>
+      <c r="M61" s="3"/>
+      <c r="N61" s="3"/>
+      <c r="O61" s="3"/>
+      <c r="P61" s="3"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="4"/>
-      <c r="B62" s="4"/>
-      <c r="C62" s="4"/>
-      <c r="D62" s="4"/>
-      <c r="E62" s="4"/>
-      <c r="F62" s="4"/>
-      <c r="G62" s="4"/>
-      <c r="H62" s="4"/>
-      <c r="I62" s="4"/>
-      <c r="J62" s="4"/>
-      <c r="K62" s="4"/>
-      <c r="L62" s="4"/>
-      <c r="M62" s="4"/>
-      <c r="N62" s="4"/>
-      <c r="O62" s="4"/>
-      <c r="P62" s="4"/>
+      <c r="A62" s="3"/>
+      <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
+      <c r="F62" s="3"/>
+      <c r="G62" s="3"/>
+      <c r="H62" s="3"/>
+      <c r="I62" s="3"/>
+      <c r="J62" s="3"/>
+      <c r="K62" s="3"/>
+      <c r="L62" s="3"/>
+      <c r="M62" s="3"/>
+      <c r="N62" s="3"/>
+      <c r="O62" s="3"/>
+      <c r="P62" s="3"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="4"/>
-      <c r="B63" s="4"/>
-      <c r="C63" s="4"/>
-      <c r="D63" s="4"/>
-      <c r="E63" s="4"/>
-      <c r="F63" s="4"/>
-      <c r="G63" s="4"/>
-      <c r="H63" s="4"/>
-      <c r="I63" s="4"/>
-      <c r="J63" s="4"/>
-      <c r="K63" s="4"/>
-      <c r="L63" s="4"/>
-      <c r="M63" s="4"/>
-      <c r="N63" s="4"/>
-      <c r="O63" s="4"/>
-      <c r="P63" s="4"/>
+      <c r="A63" s="3"/>
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3"/>
+      <c r="F63" s="3"/>
+      <c r="G63" s="3"/>
+      <c r="H63" s="3"/>
+      <c r="I63" s="3"/>
+      <c r="J63" s="3"/>
+      <c r="K63" s="3"/>
+      <c r="L63" s="3"/>
+      <c r="M63" s="3"/>
+      <c r="N63" s="3"/>
+      <c r="O63" s="3"/>
+      <c r="P63" s="3"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="4"/>
-      <c r="B64" s="4"/>
-      <c r="C64" s="4"/>
-      <c r="D64" s="4"/>
-      <c r="E64" s="4"/>
-      <c r="F64" s="4"/>
-      <c r="G64" s="4"/>
-      <c r="H64" s="4"/>
-      <c r="I64" s="4"/>
-      <c r="J64" s="4"/>
-      <c r="K64" s="4"/>
-      <c r="L64" s="4"/>
-      <c r="M64" s="4"/>
-      <c r="N64" s="4"/>
-      <c r="O64" s="4"/>
-      <c r="P64" s="4"/>
+      <c r="A64" s="3"/>
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3"/>
+      <c r="G64" s="3"/>
+      <c r="H64" s="3"/>
+      <c r="I64" s="3"/>
+      <c r="J64" s="3"/>
+      <c r="K64" s="3"/>
+      <c r="L64" s="3"/>
+      <c r="M64" s="3"/>
+      <c r="N64" s="3"/>
+      <c r="O64" s="3"/>
+      <c r="P64" s="3"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="4"/>
-      <c r="B65" s="4"/>
-      <c r="C65" s="4"/>
-      <c r="D65" s="4"/>
-      <c r="E65" s="4"/>
-      <c r="F65" s="4"/>
-      <c r="G65" s="4"/>
-      <c r="H65" s="4"/>
-      <c r="I65" s="4"/>
-      <c r="J65" s="4"/>
-      <c r="K65" s="4"/>
-      <c r="L65" s="4"/>
-      <c r="M65" s="4"/>
-      <c r="N65" s="4"/>
-      <c r="O65" s="4"/>
-      <c r="P65" s="4"/>
+      <c r="A65" s="3"/>
+      <c r="B65" s="3"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="3"/>
+      <c r="F65" s="3"/>
+      <c r="G65" s="3"/>
+      <c r="H65" s="3"/>
+      <c r="I65" s="3"/>
+      <c r="J65" s="3"/>
+      <c r="K65" s="3"/>
+      <c r="L65" s="3"/>
+      <c r="M65" s="3"/>
+      <c r="N65" s="3"/>
+      <c r="O65" s="3"/>
+      <c r="P65" s="3"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="4"/>
-      <c r="B66" s="4"/>
-      <c r="C66" s="4"/>
-      <c r="D66" s="4"/>
-      <c r="E66" s="4"/>
-      <c r="F66" s="4"/>
-      <c r="G66" s="4"/>
-      <c r="H66" s="4"/>
-      <c r="I66" s="4"/>
-      <c r="J66" s="4"/>
-      <c r="K66" s="4"/>
-      <c r="L66" s="4"/>
-      <c r="M66" s="4"/>
-      <c r="N66" s="4"/>
-      <c r="O66" s="4"/>
-      <c r="P66" s="4"/>
+      <c r="A66" s="3"/>
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+      <c r="E66" s="3"/>
+      <c r="F66" s="3"/>
+      <c r="G66" s="3"/>
+      <c r="H66" s="3"/>
+      <c r="I66" s="3"/>
+      <c r="J66" s="3"/>
+      <c r="K66" s="3"/>
+      <c r="L66" s="3"/>
+      <c r="M66" s="3"/>
+      <c r="N66" s="3"/>
+      <c r="O66" s="3"/>
+      <c r="P66" s="3"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="4"/>
-      <c r="B67" s="4"/>
-      <c r="C67" s="4"/>
-      <c r="D67" s="4"/>
-      <c r="E67" s="4"/>
-      <c r="F67" s="4"/>
-      <c r="G67" s="4"/>
-      <c r="H67" s="4"/>
-      <c r="I67" s="4"/>
-      <c r="J67" s="4"/>
-      <c r="K67" s="4"/>
-      <c r="L67" s="4"/>
-      <c r="M67" s="4"/>
-      <c r="N67" s="4"/>
-      <c r="O67" s="4"/>
-      <c r="P67" s="4"/>
+      <c r="A67" s="3"/>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3"/>
+      <c r="F67" s="3"/>
+      <c r="G67" s="3"/>
+      <c r="H67" s="3"/>
+      <c r="I67" s="3"/>
+      <c r="J67" s="3"/>
+      <c r="K67" s="3"/>
+      <c r="L67" s="3"/>
+      <c r="M67" s="3"/>
+      <c r="N67" s="3"/>
+      <c r="O67" s="3"/>
+      <c r="P67" s="3"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="4"/>
-      <c r="B68" s="4"/>
-      <c r="C68" s="4"/>
-      <c r="D68" s="4"/>
-      <c r="E68" s="4"/>
-      <c r="F68" s="4"/>
-      <c r="G68" s="4"/>
-      <c r="H68" s="4"/>
-      <c r="I68" s="4"/>
-      <c r="J68" s="4"/>
-      <c r="K68" s="4"/>
-      <c r="L68" s="4"/>
-      <c r="M68" s="4"/>
-      <c r="N68" s="4"/>
-      <c r="O68" s="4"/>
-      <c r="P68" s="4"/>
+      <c r="A68" s="3"/>
+      <c r="B68" s="3"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3"/>
+      <c r="F68" s="3"/>
+      <c r="G68" s="3"/>
+      <c r="H68" s="3"/>
+      <c r="I68" s="3"/>
+      <c r="J68" s="3"/>
+      <c r="K68" s="3"/>
+      <c r="L68" s="3"/>
+      <c r="M68" s="3"/>
+      <c r="N68" s="3"/>
+      <c r="O68" s="3"/>
+      <c r="P68" s="3"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="4"/>
-      <c r="B69" s="4"/>
-      <c r="C69" s="4"/>
-      <c r="D69" s="4"/>
-      <c r="E69" s="4"/>
-      <c r="F69" s="4"/>
-      <c r="G69" s="4"/>
-      <c r="H69" s="4"/>
-      <c r="I69" s="4"/>
-      <c r="J69" s="4"/>
-      <c r="K69" s="4"/>
-      <c r="L69" s="4"/>
-      <c r="M69" s="4"/>
-      <c r="N69" s="4"/>
-      <c r="O69" s="4"/>
-      <c r="P69" s="4"/>
+      <c r="A69" s="3"/>
+      <c r="B69" s="3"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+      <c r="E69" s="3"/>
+      <c r="F69" s="3"/>
+      <c r="G69" s="3"/>
+      <c r="H69" s="3"/>
+      <c r="I69" s="3"/>
+      <c r="J69" s="3"/>
+      <c r="K69" s="3"/>
+      <c r="L69" s="3"/>
+      <c r="M69" s="3"/>
+      <c r="N69" s="3"/>
+      <c r="O69" s="3"/>
+      <c r="P69" s="3"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="4"/>
-      <c r="B70" s="4"/>
-      <c r="C70" s="4"/>
-      <c r="D70" s="4"/>
-      <c r="E70" s="4"/>
-      <c r="F70" s="4"/>
-      <c r="G70" s="4"/>
-      <c r="H70" s="4"/>
-      <c r="I70" s="4"/>
-      <c r="J70" s="4"/>
-      <c r="K70" s="4"/>
-      <c r="L70" s="4"/>
-      <c r="M70" s="4"/>
-      <c r="N70" s="4"/>
-      <c r="O70" s="4"/>
-      <c r="P70" s="4"/>
+      <c r="A70" s="3"/>
+      <c r="B70" s="3"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="3"/>
+      <c r="G70" s="3"/>
+      <c r="H70" s="3"/>
+      <c r="I70" s="3"/>
+      <c r="J70" s="3"/>
+      <c r="K70" s="3"/>
+      <c r="L70" s="3"/>
+      <c r="M70" s="3"/>
+      <c r="N70" s="3"/>
+      <c r="O70" s="3"/>
+      <c r="P70" s="3"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="4"/>
-      <c r="B71" s="4"/>
-      <c r="C71" s="4"/>
-      <c r="D71" s="4"/>
-      <c r="E71" s="4"/>
-      <c r="F71" s="4"/>
-      <c r="G71" s="4"/>
-      <c r="H71" s="4"/>
-      <c r="I71" s="4"/>
-      <c r="J71" s="4"/>
-      <c r="K71" s="4"/>
-      <c r="L71" s="4"/>
-      <c r="M71" s="4"/>
-      <c r="N71" s="4"/>
-      <c r="O71" s="4"/>
-      <c r="P71" s="4"/>
+      <c r="A71" s="3"/>
+      <c r="B71" s="3"/>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="3"/>
+      <c r="F71" s="3"/>
+      <c r="G71" s="3"/>
+      <c r="H71" s="3"/>
+      <c r="I71" s="3"/>
+      <c r="J71" s="3"/>
+      <c r="K71" s="3"/>
+      <c r="L71" s="3"/>
+      <c r="M71" s="3"/>
+      <c r="N71" s="3"/>
+      <c r="O71" s="3"/>
+      <c r="P71" s="3"/>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="4"/>
-      <c r="B72" s="4"/>
-      <c r="C72" s="4"/>
-      <c r="D72" s="4"/>
-      <c r="E72" s="4"/>
-      <c r="F72" s="4"/>
-      <c r="G72" s="4"/>
-      <c r="H72" s="4"/>
-      <c r="I72" s="4"/>
-      <c r="J72" s="4"/>
-      <c r="K72" s="4"/>
-      <c r="L72" s="4"/>
-      <c r="M72" s="4"/>
-      <c r="N72" s="4"/>
-      <c r="O72" s="4"/>
-      <c r="P72" s="4"/>
+      <c r="A72" s="3"/>
+      <c r="B72" s="3"/>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+      <c r="E72" s="3"/>
+      <c r="F72" s="3"/>
+      <c r="G72" s="3"/>
+      <c r="H72" s="3"/>
+      <c r="I72" s="3"/>
+      <c r="J72" s="3"/>
+      <c r="K72" s="3"/>
+      <c r="L72" s="3"/>
+      <c r="M72" s="3"/>
+      <c r="N72" s="3"/>
+      <c r="O72" s="3"/>
+      <c r="P72" s="3"/>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="4"/>
-      <c r="B73" s="4"/>
-      <c r="C73" s="4"/>
-      <c r="D73" s="4"/>
-      <c r="E73" s="4"/>
-      <c r="F73" s="4"/>
-      <c r="G73" s="4"/>
-      <c r="H73" s="4"/>
-      <c r="I73" s="4"/>
-      <c r="J73" s="4"/>
-      <c r="K73" s="4"/>
-      <c r="L73" s="4"/>
-      <c r="M73" s="4"/>
-      <c r="N73" s="4"/>
-      <c r="O73" s="4"/>
-      <c r="P73" s="4"/>
+      <c r="A73" s="3"/>
+      <c r="B73" s="3"/>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="3"/>
+      <c r="F73" s="3"/>
+      <c r="G73" s="3"/>
+      <c r="H73" s="3"/>
+      <c r="I73" s="3"/>
+      <c r="J73" s="3"/>
+      <c r="K73" s="3"/>
+      <c r="L73" s="3"/>
+      <c r="M73" s="3"/>
+      <c r="N73" s="3"/>
+      <c r="O73" s="3"/>
+      <c r="P73" s="3"/>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="4"/>
-      <c r="B74" s="4"/>
-      <c r="C74" s="4"/>
-      <c r="D74" s="4"/>
-      <c r="E74" s="4"/>
-      <c r="F74" s="4"/>
-      <c r="G74" s="4"/>
-      <c r="H74" s="4"/>
-      <c r="I74" s="4"/>
-      <c r="J74" s="4"/>
-      <c r="K74" s="4"/>
-      <c r="L74" s="4"/>
-      <c r="M74" s="4"/>
-      <c r="N74" s="4"/>
-      <c r="O74" s="4"/>
-      <c r="P74" s="4"/>
+      <c r="A74" s="3"/>
+      <c r="B74" s="3"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+      <c r="E74" s="3"/>
+      <c r="F74" s="3"/>
+      <c r="G74" s="3"/>
+      <c r="H74" s="3"/>
+      <c r="I74" s="3"/>
+      <c r="J74" s="3"/>
+      <c r="K74" s="3"/>
+      <c r="L74" s="3"/>
+      <c r="M74" s="3"/>
+      <c r="N74" s="3"/>
+      <c r="O74" s="3"/>
+      <c r="P74" s="3"/>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="4"/>
-      <c r="B75" s="4"/>
-      <c r="C75" s="4"/>
-      <c r="D75" s="4"/>
-      <c r="E75" s="4"/>
-      <c r="F75" s="4"/>
-      <c r="G75" s="4"/>
-      <c r="H75" s="4"/>
-      <c r="I75" s="4"/>
-      <c r="J75" s="4"/>
-      <c r="K75" s="4"/>
-      <c r="L75" s="4"/>
-      <c r="M75" s="4"/>
-      <c r="N75" s="4"/>
-      <c r="O75" s="4"/>
-      <c r="P75" s="4"/>
+      <c r="A75" s="3"/>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="3"/>
+      <c r="G75" s="3"/>
+      <c r="H75" s="3"/>
+      <c r="I75" s="3"/>
+      <c r="J75" s="3"/>
+      <c r="K75" s="3"/>
+      <c r="L75" s="3"/>
+      <c r="M75" s="3"/>
+      <c r="N75" s="3"/>
+      <c r="O75" s="3"/>
+      <c r="P75" s="3"/>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="4"/>
-      <c r="B76" s="4"/>
-      <c r="C76" s="4"/>
-      <c r="D76" s="4"/>
-      <c r="E76" s="4"/>
-      <c r="F76" s="4"/>
-      <c r="G76" s="4"/>
-      <c r="H76" s="4"/>
-      <c r="I76" s="4"/>
-      <c r="J76" s="4"/>
-      <c r="K76" s="4"/>
-      <c r="L76" s="4"/>
-      <c r="M76" s="4"/>
-      <c r="N76" s="4"/>
-      <c r="O76" s="4"/>
-      <c r="P76" s="4"/>
+      <c r="A76" s="3"/>
+      <c r="B76" s="3"/>
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="3"/>
+      <c r="G76" s="3"/>
+      <c r="H76" s="3"/>
+      <c r="I76" s="3"/>
+      <c r="J76" s="3"/>
+      <c r="K76" s="3"/>
+      <c r="L76" s="3"/>
+      <c r="M76" s="3"/>
+      <c r="N76" s="3"/>
+      <c r="O76" s="3"/>
+      <c r="P76" s="3"/>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="4"/>
-      <c r="B77" s="4"/>
-      <c r="C77" s="4"/>
-      <c r="D77" s="4"/>
-      <c r="E77" s="4"/>
-      <c r="F77" s="4"/>
-      <c r="G77" s="4"/>
-      <c r="H77" s="4"/>
-      <c r="I77" s="4"/>
-      <c r="J77" s="4"/>
-      <c r="K77" s="4"/>
-      <c r="L77" s="4"/>
-      <c r="M77" s="4"/>
-      <c r="N77" s="4"/>
-      <c r="O77" s="4"/>
-      <c r="P77" s="4"/>
+      <c r="A77" s="3"/>
+      <c r="B77" s="3"/>
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
+      <c r="E77" s="3"/>
+      <c r="F77" s="3"/>
+      <c r="G77" s="3"/>
+      <c r="H77" s="3"/>
+      <c r="I77" s="3"/>
+      <c r="J77" s="3"/>
+      <c r="K77" s="3"/>
+      <c r="L77" s="3"/>
+      <c r="M77" s="3"/>
+      <c r="N77" s="3"/>
+      <c r="O77" s="3"/>
+      <c r="P77" s="3"/>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="4"/>
-      <c r="B78" s="4"/>
-      <c r="C78" s="4"/>
-      <c r="D78" s="4"/>
-      <c r="E78" s="4"/>
-      <c r="F78" s="4"/>
-      <c r="G78" s="4"/>
-      <c r="H78" s="4"/>
-      <c r="I78" s="4"/>
-      <c r="J78" s="4"/>
-      <c r="K78" s="4"/>
-      <c r="L78" s="4"/>
-      <c r="M78" s="4"/>
-      <c r="N78" s="4"/>
-      <c r="O78" s="4"/>
-      <c r="P78" s="4"/>
+      <c r="A78" s="3"/>
+      <c r="B78" s="3"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="3"/>
+      <c r="E78" s="3"/>
+      <c r="F78" s="3"/>
+      <c r="G78" s="3"/>
+      <c r="H78" s="3"/>
+      <c r="I78" s="3"/>
+      <c r="J78" s="3"/>
+      <c r="K78" s="3"/>
+      <c r="L78" s="3"/>
+      <c r="M78" s="3"/>
+      <c r="N78" s="3"/>
+      <c r="O78" s="3"/>
+      <c r="P78" s="3"/>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="4"/>
-      <c r="B79" s="4"/>
-      <c r="C79" s="4"/>
-      <c r="D79" s="4"/>
-      <c r="E79" s="4"/>
-      <c r="F79" s="4"/>
-      <c r="G79" s="4"/>
-      <c r="H79" s="4"/>
-      <c r="I79" s="4"/>
-      <c r="J79" s="4"/>
-      <c r="K79" s="4"/>
-      <c r="L79" s="4"/>
-      <c r="M79" s="4"/>
-      <c r="N79" s="4"/>
-      <c r="O79" s="4"/>
-      <c r="P79" s="4"/>
+      <c r="A79" s="3"/>
+      <c r="B79" s="3"/>
+      <c r="C79" s="3"/>
+      <c r="D79" s="3"/>
+      <c r="E79" s="3"/>
+      <c r="F79" s="3"/>
+      <c r="G79" s="3"/>
+      <c r="H79" s="3"/>
+      <c r="I79" s="3"/>
+      <c r="J79" s="3"/>
+      <c r="K79" s="3"/>
+      <c r="L79" s="3"/>
+      <c r="M79" s="3"/>
+      <c r="N79" s="3"/>
+      <c r="O79" s="3"/>
+      <c r="P79" s="3"/>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="4"/>
-      <c r="B80" s="4"/>
-      <c r="C80" s="4"/>
-      <c r="D80" s="4"/>
-      <c r="E80" s="4"/>
-      <c r="F80" s="4"/>
-      <c r="G80" s="4"/>
-      <c r="H80" s="4"/>
-      <c r="I80" s="4"/>
-      <c r="J80" s="4"/>
-      <c r="K80" s="4"/>
-      <c r="L80" s="4"/>
-      <c r="M80" s="4"/>
-      <c r="N80" s="4"/>
-      <c r="O80" s="4"/>
-      <c r="P80" s="4"/>
+      <c r="A80" s="3"/>
+      <c r="B80" s="3"/>
+      <c r="C80" s="3"/>
+      <c r="D80" s="3"/>
+      <c r="E80" s="3"/>
+      <c r="F80" s="3"/>
+      <c r="G80" s="3"/>
+      <c r="H80" s="3"/>
+      <c r="I80" s="3"/>
+      <c r="J80" s="3"/>
+      <c r="K80" s="3"/>
+      <c r="L80" s="3"/>
+      <c r="M80" s="3"/>
+      <c r="N80" s="3"/>
+      <c r="O80" s="3"/>
+      <c r="P80" s="3"/>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="4"/>
-      <c r="B81" s="4"/>
-      <c r="C81" s="4"/>
-      <c r="D81" s="4"/>
-      <c r="E81" s="4"/>
-      <c r="F81" s="4"/>
-      <c r="G81" s="4"/>
-      <c r="H81" s="4"/>
-      <c r="I81" s="4"/>
-      <c r="J81" s="4"/>
-      <c r="K81" s="4"/>
-      <c r="L81" s="4"/>
-      <c r="M81" s="4"/>
-      <c r="N81" s="4"/>
-      <c r="O81" s="4"/>
-      <c r="P81" s="4"/>
+      <c r="A81" s="3"/>
+      <c r="B81" s="3"/>
+      <c r="C81" s="3"/>
+      <c r="D81" s="3"/>
+      <c r="E81" s="3"/>
+      <c r="F81" s="3"/>
+      <c r="G81" s="3"/>
+      <c r="H81" s="3"/>
+      <c r="I81" s="3"/>
+      <c r="J81" s="3"/>
+      <c r="K81" s="3"/>
+      <c r="L81" s="3"/>
+      <c r="M81" s="3"/>
+      <c r="N81" s="3"/>
+      <c r="O81" s="3"/>
+      <c r="P81" s="3"/>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="4"/>
-      <c r="B82" s="4"/>
-      <c r="C82" s="4"/>
-      <c r="D82" s="4"/>
-      <c r="E82" s="4"/>
-      <c r="F82" s="4"/>
-      <c r="G82" s="4"/>
-      <c r="H82" s="4"/>
-      <c r="I82" s="4"/>
-      <c r="J82" s="4"/>
-      <c r="K82" s="4"/>
-      <c r="L82" s="4"/>
-      <c r="M82" s="4"/>
-      <c r="N82" s="4"/>
-      <c r="O82" s="4"/>
-      <c r="P82" s="4"/>
+      <c r="A82" s="3"/>
+      <c r="B82" s="3"/>
+      <c r="C82" s="3"/>
+      <c r="D82" s="3"/>
+      <c r="E82" s="3"/>
+      <c r="F82" s="3"/>
+      <c r="G82" s="3"/>
+      <c r="H82" s="3"/>
+      <c r="I82" s="3"/>
+      <c r="J82" s="3"/>
+      <c r="K82" s="3"/>
+      <c r="L82" s="3"/>
+      <c r="M82" s="3"/>
+      <c r="N82" s="3"/>
+      <c r="O82" s="3"/>
+      <c r="P82" s="3"/>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="4"/>
-      <c r="B83" s="4"/>
-      <c r="C83" s="4"/>
-      <c r="D83" s="4"/>
-      <c r="E83" s="4"/>
-      <c r="F83" s="4"/>
-      <c r="G83" s="4"/>
-      <c r="H83" s="4"/>
-      <c r="I83" s="4"/>
-      <c r="J83" s="4"/>
-      <c r="K83" s="4"/>
-      <c r="L83" s="4"/>
-      <c r="M83" s="4"/>
-      <c r="N83" s="4"/>
-      <c r="O83" s="4"/>
-      <c r="P83" s="4"/>
+      <c r="A83" s="3"/>
+      <c r="B83" s="3"/>
+      <c r="C83" s="3"/>
+      <c r="D83" s="3"/>
+      <c r="E83" s="3"/>
+      <c r="F83" s="3"/>
+      <c r="G83" s="3"/>
+      <c r="H83" s="3"/>
+      <c r="I83" s="3"/>
+      <c r="J83" s="3"/>
+      <c r="K83" s="3"/>
+      <c r="L83" s="3"/>
+      <c r="M83" s="3"/>
+      <c r="N83" s="3"/>
+      <c r="O83" s="3"/>
+      <c r="P83" s="3"/>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="4"/>
-      <c r="B84" s="4"/>
-      <c r="C84" s="4"/>
-      <c r="D84" s="4"/>
-      <c r="E84" s="4"/>
-      <c r="F84" s="4"/>
-      <c r="G84" s="4"/>
-      <c r="H84" s="4"/>
-      <c r="I84" s="4"/>
-      <c r="J84" s="4"/>
-      <c r="K84" s="4"/>
-      <c r="L84" s="4"/>
-      <c r="M84" s="4"/>
-      <c r="N84" s="4"/>
-      <c r="O84" s="4"/>
-      <c r="P84" s="4"/>
+      <c r="A84" s="3"/>
+      <c r="B84" s="3"/>
+      <c r="C84" s="3"/>
+      <c r="D84" s="3"/>
+      <c r="E84" s="3"/>
+      <c r="F84" s="3"/>
+      <c r="G84" s="3"/>
+      <c r="H84" s="3"/>
+      <c r="I84" s="3"/>
+      <c r="J84" s="3"/>
+      <c r="K84" s="3"/>
+      <c r="L84" s="3"/>
+      <c r="M84" s="3"/>
+      <c r="N84" s="3"/>
+      <c r="O84" s="3"/>
+      <c r="P84" s="3"/>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="4"/>
-      <c r="B85" s="4"/>
-      <c r="C85" s="4"/>
-      <c r="D85" s="4"/>
-      <c r="E85" s="4"/>
-      <c r="F85" s="4"/>
-      <c r="G85" s="4"/>
-      <c r="H85" s="4"/>
-      <c r="I85" s="4"/>
-      <c r="J85" s="4"/>
-      <c r="K85" s="4"/>
-      <c r="L85" s="4"/>
-      <c r="M85" s="4"/>
-      <c r="N85" s="4"/>
-      <c r="O85" s="4"/>
-      <c r="P85" s="4"/>
+      <c r="A85" s="3"/>
+      <c r="B85" s="3"/>
+      <c r="C85" s="3"/>
+      <c r="D85" s="3"/>
+      <c r="E85" s="3"/>
+      <c r="F85" s="3"/>
+      <c r="G85" s="3"/>
+      <c r="H85" s="3"/>
+      <c r="I85" s="3"/>
+      <c r="J85" s="3"/>
+      <c r="K85" s="3"/>
+      <c r="L85" s="3"/>
+      <c r="M85" s="3"/>
+      <c r="N85" s="3"/>
+      <c r="O85" s="3"/>
+      <c r="P85" s="3"/>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="4"/>
-      <c r="B86" s="4"/>
-      <c r="C86" s="4"/>
-      <c r="D86" s="4"/>
-      <c r="E86" s="4"/>
-      <c r="F86" s="4"/>
-      <c r="G86" s="4"/>
-      <c r="H86" s="4"/>
-      <c r="I86" s="4"/>
-      <c r="J86" s="4"/>
-      <c r="K86" s="4"/>
-      <c r="L86" s="4"/>
-      <c r="M86" s="4"/>
-      <c r="N86" s="4"/>
-      <c r="O86" s="4"/>
-      <c r="P86" s="4"/>
+      <c r="A86" s="3"/>
+      <c r="B86" s="3"/>
+      <c r="C86" s="3"/>
+      <c r="D86" s="3"/>
+      <c r="E86" s="3"/>
+      <c r="F86" s="3"/>
+      <c r="G86" s="3"/>
+      <c r="H86" s="3"/>
+      <c r="I86" s="3"/>
+      <c r="J86" s="3"/>
+      <c r="K86" s="3"/>
+      <c r="L86" s="3"/>
+      <c r="M86" s="3"/>
+      <c r="N86" s="3"/>
+      <c r="O86" s="3"/>
+      <c r="P86" s="3"/>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="4"/>
-      <c r="B87" s="4"/>
-      <c r="C87" s="4"/>
-      <c r="D87" s="4"/>
-      <c r="E87" s="4"/>
-      <c r="F87" s="4"/>
-      <c r="G87" s="4"/>
-      <c r="H87" s="4"/>
-      <c r="I87" s="4"/>
-      <c r="J87" s="4"/>
-      <c r="K87" s="4"/>
-      <c r="L87" s="4"/>
-      <c r="M87" s="4"/>
-      <c r="N87" s="4"/>
-      <c r="O87" s="4"/>
-      <c r="P87" s="4"/>
+      <c r="A87" s="3"/>
+      <c r="B87" s="3"/>
+      <c r="C87" s="3"/>
+      <c r="D87" s="3"/>
+      <c r="E87" s="3"/>
+      <c r="F87" s="3"/>
+      <c r="G87" s="3"/>
+      <c r="H87" s="3"/>
+      <c r="I87" s="3"/>
+      <c r="J87" s="3"/>
+      <c r="K87" s="3"/>
+      <c r="L87" s="3"/>
+      <c r="M87" s="3"/>
+      <c r="N87" s="3"/>
+      <c r="O87" s="3"/>
+      <c r="P87" s="3"/>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="4"/>
-      <c r="B88" s="4"/>
-      <c r="C88" s="4"/>
-      <c r="D88" s="4"/>
-      <c r="E88" s="4"/>
-      <c r="F88" s="4"/>
-      <c r="G88" s="4"/>
-      <c r="H88" s="4"/>
-      <c r="I88" s="4"/>
-      <c r="J88" s="4"/>
-      <c r="K88" s="4"/>
-      <c r="L88" s="4"/>
-      <c r="M88" s="4"/>
-      <c r="N88" s="4"/>
-      <c r="O88" s="4"/>
-      <c r="P88" s="4"/>
+      <c r="A88" s="3"/>
+      <c r="B88" s="3"/>
+      <c r="C88" s="3"/>
+      <c r="D88" s="3"/>
+      <c r="E88" s="3"/>
+      <c r="F88" s="3"/>
+      <c r="G88" s="3"/>
+      <c r="H88" s="3"/>
+      <c r="I88" s="3"/>
+      <c r="J88" s="3"/>
+      <c r="K88" s="3"/>
+      <c r="L88" s="3"/>
+      <c r="M88" s="3"/>
+      <c r="N88" s="3"/>
+      <c r="O88" s="3"/>
+      <c r="P88" s="3"/>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="4"/>
-      <c r="B89" s="4"/>
-      <c r="C89" s="4"/>
-      <c r="D89" s="4"/>
-      <c r="E89" s="4"/>
-      <c r="F89" s="4"/>
-      <c r="G89" s="4"/>
-      <c r="H89" s="4"/>
-      <c r="I89" s="4"/>
-      <c r="J89" s="4"/>
-      <c r="K89" s="4"/>
-      <c r="L89" s="4"/>
-      <c r="M89" s="4"/>
-      <c r="N89" s="4"/>
-      <c r="O89" s="4"/>
-      <c r="P89" s="4"/>
+      <c r="A89" s="3"/>
+      <c r="B89" s="3"/>
+      <c r="C89" s="3"/>
+      <c r="D89" s="3"/>
+      <c r="E89" s="3"/>
+      <c r="F89" s="3"/>
+      <c r="G89" s="3"/>
+      <c r="H89" s="3"/>
+      <c r="I89" s="3"/>
+      <c r="J89" s="3"/>
+      <c r="K89" s="3"/>
+      <c r="L89" s="3"/>
+      <c r="M89" s="3"/>
+      <c r="N89" s="3"/>
+      <c r="O89" s="3"/>
+      <c r="P89" s="3"/>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="4"/>
-      <c r="B90" s="4"/>
-      <c r="C90" s="4"/>
-      <c r="D90" s="4"/>
-      <c r="E90" s="4"/>
-      <c r="F90" s="4"/>
-      <c r="G90" s="4"/>
-      <c r="H90" s="4"/>
-      <c r="I90" s="4"/>
-      <c r="J90" s="4"/>
-      <c r="K90" s="4"/>
-      <c r="L90" s="4"/>
-      <c r="M90" s="4"/>
-      <c r="N90" s="4"/>
-      <c r="O90" s="4"/>
-      <c r="P90" s="4"/>
+      <c r="A90" s="3"/>
+      <c r="B90" s="3"/>
+      <c r="C90" s="3"/>
+      <c r="D90" s="3"/>
+      <c r="E90" s="3"/>
+      <c r="F90" s="3"/>
+      <c r="G90" s="3"/>
+      <c r="H90" s="3"/>
+      <c r="I90" s="3"/>
+      <c r="J90" s="3"/>
+      <c r="K90" s="3"/>
+      <c r="L90" s="3"/>
+      <c r="M90" s="3"/>
+      <c r="N90" s="3"/>
+      <c r="O90" s="3"/>
+      <c r="P90" s="3"/>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="4"/>
-      <c r="B91" s="4"/>
-      <c r="C91" s="4"/>
-      <c r="D91" s="4"/>
-      <c r="E91" s="4"/>
-      <c r="F91" s="4"/>
-      <c r="G91" s="4"/>
-      <c r="H91" s="4"/>
-      <c r="I91" s="4"/>
-      <c r="J91" s="4"/>
-      <c r="K91" s="4"/>
-      <c r="L91" s="4"/>
-      <c r="M91" s="4"/>
-      <c r="N91" s="4"/>
-      <c r="O91" s="4"/>
-      <c r="P91" s="4"/>
+      <c r="A91" s="3"/>
+      <c r="B91" s="3"/>
+      <c r="C91" s="3"/>
+      <c r="D91" s="3"/>
+      <c r="E91" s="3"/>
+      <c r="F91" s="3"/>
+      <c r="G91" s="3"/>
+      <c r="H91" s="3"/>
+      <c r="I91" s="3"/>
+      <c r="J91" s="3"/>
+      <c r="K91" s="3"/>
+      <c r="L91" s="3"/>
+      <c r="M91" s="3"/>
+      <c r="N91" s="3"/>
+      <c r="O91" s="3"/>
+      <c r="P91" s="3"/>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E95" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>